<commit_message>
Log updated and Marketing plan is in progress
Log updated and Marketing plan is in progress
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Information/LogBook/Log-Debashish-Nath.xlsx
+++ b/Offline/BusinessManagement/Information/LogBook/Log-Debashish-Nath.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\LogBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EB34C5-FC0E-41BB-8E45-A883DE645E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C418B86-00F7-4FFF-A102-1BCA761BFD66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>SlNo</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Updated Ops for October -2023</t>
   </si>
   <si>
-    <t>Partial</t>
-  </si>
-  <si>
     <t>Remarks</t>
   </si>
   <si>
@@ -60,10 +57,37 @@
     <t>Got Physics,Chemistry and Maths syllabus from Sahesta of JELET Crash Course</t>
   </si>
   <si>
-    <t>Subroto Ghosh needs to give topics covered on 19th October. He will send in evening</t>
-  </si>
-  <si>
     <t>Format of metrics related to syllabus of each subject coverage</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Mock Test Planning</t>
+  </si>
+  <si>
+    <t>Called Waqar Younis and Manpreet of College Doors but they did n't picked up the call</t>
+  </si>
+  <si>
+    <t>Connected with Waqar Younis of College Doors about Mock Exam</t>
+  </si>
+  <si>
+    <t>Talked with Mr Subroto Ghosh for practice test</t>
+  </si>
+  <si>
+    <t>Sayan took my AI class for 2 hours</t>
+  </si>
+  <si>
+    <t>Called Mr Subroto Ghosh and he said he will update the note details in night</t>
+  </si>
+  <si>
+    <t>For JILETE we need to purchase question bank and for Prottoy we need to talk with his father which test he wants to give board level or joint</t>
+  </si>
+  <si>
+    <t>Talked with Mr Amitabha Kairali for Prottoy's monthly test</t>
+  </si>
+  <si>
+    <t>As Prottoy will give JEE and JEE WB exams, hence he will give practice test on this exams.</t>
   </si>
 </sst>
 </file>
@@ -397,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,7 +432,8 @@
     <col min="1" max="1" width="4.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="101.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -425,7 +450,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -439,10 +464,10 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -456,7 +481,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -467,10 +492,10 @@
         <v>45229</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -481,10 +506,10 @@
         <v>45229</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -495,7 +520,89 @@
         <v>45229</v>
       </c>
       <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45229</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45230</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45230</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45230</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>45230</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>